<commit_message>
VR lab programme material rendering. without envelopping anchor
</commit_message>
<xml_diff>
--- a/programme-material-rendering/VR-lab_info/channel_map.xlsx
+++ b/programme-material-rendering/VR-lab_info/channel_map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://beotalk-my.sharepoint.com/personal/feig_bang-olufsen_dk/Documents/Next Generation Audio SA/Special Course/Three Driver Speaker arrangement to improve spatial awareness/Development/Special-Project/rendering-scripts/VR-lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://beotalk-my.sharepoint.com/personal/feig_bang-olufsen_dk/Documents/Next Generation Audio SA/Special Course/Perceptual-Evaluation-of-Irregular-Loudspeakers-Array/Development/Special-Project/rendering-scripts/VR-lab_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="560" documentId="8_{40E2C52F-768F-4760-9861-7CEB0A0671FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8D78FED-689D-420F-B469-38FD07FEBBD3}"/>
+  <xr:revisionPtr revIDLastSave="565" documentId="8_{40E2C52F-768F-4760-9861-7CEB0A0671FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B026E9D8-3516-4C6B-8B55-88869194D992}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="36">
   <si>
     <t>Chn_AVIL</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Chn_VRlab</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -867,10 +870,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6061940A-0730-4801-BFAE-356B925AE883}" name="Table1" displayName="Table1" ref="D8:H72" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17">
   <autoFilter ref="D8:H72" xr:uid="{6061940A-0730-4801-BFAE-356B925AE883}"/>
@@ -890,7 +889,7 @@
   <autoFilter ref="J1:L50" xr:uid="{DF83E601-0105-427F-9FBC-3048D8265312}">
     <filterColumn colId="2">
       <filters>
-        <filter val="30"/>
+        <filter val="0"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2921,7 +2920,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2989,7 +2988,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3018,7 +3017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3047,7 +3046,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3105,7 +3104,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3221,7 +3220,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3250,7 +3249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3279,7 +3278,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3387,7 +3386,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3437,7 +3436,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3466,7 +3465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3524,7 +3523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="26">
         <v>21</v>
       </c>
@@ -3582,7 +3581,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="26">
         <v>23</v>
       </c>
@@ -3611,7 +3610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="26">
         <v>24</v>
       </c>
@@ -3640,7 +3639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="26">
         <v>25</v>
       </c>
@@ -3698,7 +3697,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="26">
         <v>27</v>
       </c>
@@ -3723,7 +3722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="26">
         <v>28</v>
       </c>
@@ -3744,7 +3743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="26">
         <v>29</v>
       </c>
@@ -3786,7 +3785,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="26">
         <v>31</v>
       </c>
@@ -3807,7 +3806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="26">
         <v>32</v>
       </c>
@@ -3828,7 +3827,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J34" s="30">
         <v>40</v>
       </c>
@@ -3861,7 +3860,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J37" s="30">
         <v>43</v>
       </c>
@@ -3872,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="J38" s="30">
         <v>44</v>
       </c>
@@ -3883,7 +3882,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J39" s="29">
         <v>45</v>
       </c>
@@ -3916,7 +3915,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J42" s="29">
         <v>51</v>
       </c>
@@ -3938,7 +3937,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J44" s="30">
         <v>53</v>
       </c>
@@ -3949,7 +3948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="J45" s="30">
         <v>54</v>
       </c>
@@ -3982,9 +3981,9 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
-      <c r="J48" s="30">
-        <v>57</v>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J48" s="30" t="s">
+        <v>35</v>
       </c>
       <c r="K48" s="26">
         <v>-30</v>
@@ -4004,7 +4003,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="10:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:12" x14ac:dyDescent="0.35">
       <c r="J50" s="36">
         <v>59</v>
       </c>

</xml_diff>